<commit_message>
updated the data for 15 and 16th may
</commit_message>
<xml_diff>
--- a/02062025-delhi-aiims-bsc-nursing-prepatory-data-set.xlsx
+++ b/02062025-delhi-aiims-bsc-nursing-prepatory-data-set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Github\student_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D74C422-0B52-46FD-9264-C790CFB53263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40D670F-0A20-49AC-83E4-FD3A96F93C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A5A00A1E-0852-4B43-B760-DC16954E0468}"/>
   </bookViews>
@@ -6477,8 +6477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345E9B88-8FA7-480F-BC36-23D2BE33213E}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7716,37 +7716,45 @@
       <c r="C25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="7" t="str">
+      <c r="D25" s="5">
+        <v>50</v>
+      </c>
+      <c r="E25" s="5">
+        <v>46</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
+        <v>4</v>
+      </c>
+      <c r="H25" s="7">
         <f t="shared" ref="H25:H29" si="9">IF(AND(ISNUMBER(E25), ISNUMBER(F25), ISNUMBER(G25)), E25 - (F25* 1/3), "")</f>
-        <v/>
+        <v>46</v>
       </c>
       <c r="I25" s="5">
         <f t="shared" ref="I25:I29" si="10">D25*1</f>
+        <v>50</v>
+      </c>
+      <c r="J25" s="7">
+        <f t="shared" si="8"/>
+        <v>92</v>
+      </c>
+      <c r="K25" s="7">
+        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
+        <v>27.6</v>
+      </c>
+      <c r="L25" s="6">
+        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
+        <v>0.92</v>
+      </c>
+      <c r="M25" s="6">
+        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
+        <v>0.92</v>
+      </c>
+      <c r="N25" s="6">
+        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
         <v>0</v>
-      </c>
-      <c r="J25" s="7" t="e">
-        <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K25" s="7" t="e">
-        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L25" s="6" t="e">
-        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25" s="6" t="e">
-        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N25" s="6" t="e">
-        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
@@ -7808,37 +7816,45 @@
       <c r="C27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="7" t="str">
+      <c r="D27" s="5">
+        <v>25</v>
+      </c>
+      <c r="E27" s="5">
+        <v>23</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>2</v>
+      </c>
+      <c r="H27" s="7">
         <f t="shared" si="9"/>
-        <v/>
+        <v>23</v>
       </c>
       <c r="I27" s="5">
         <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="J27" s="7">
+        <f t="shared" si="8"/>
+        <v>92</v>
+      </c>
+      <c r="K27" s="7">
+        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
+        <v>27.6</v>
+      </c>
+      <c r="L27" s="6">
+        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
+        <v>0.92</v>
+      </c>
+      <c r="M27" s="6">
+        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
+        <v>0.92</v>
+      </c>
+      <c r="N27" s="6">
+        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
         <v>0</v>
-      </c>
-      <c r="J27" s="7" t="e">
-        <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K27" s="7" t="e">
-        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L27" s="6" t="e">
-        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M27" s="6" t="e">
-        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N27" s="6" t="e">
-        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -7849,37 +7865,45 @@
       <c r="C28" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="7" t="str">
+      <c r="D28" s="5">
+        <v>50</v>
+      </c>
+      <c r="E28" s="5">
+        <v>49</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+      <c r="H28" s="7">
         <f t="shared" si="9"/>
-        <v/>
+        <v>49</v>
       </c>
       <c r="I28" s="5">
         <f t="shared" si="10"/>
+        <v>50</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="8"/>
+        <v>98</v>
+      </c>
+      <c r="K28" s="7">
+        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
+        <v>29.4</v>
+      </c>
+      <c r="L28" s="6">
+        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
+        <v>0.98</v>
+      </c>
+      <c r="M28" s="6">
+        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
+        <v>0.98</v>
+      </c>
+      <c r="N28" s="6">
+        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
         <v>0</v>
-      </c>
-      <c r="J28" s="7" t="e">
-        <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K28" s="7" t="e">
-        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L28" s="6" t="e">
-        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M28" s="6" t="e">
-        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N28" s="6" t="e">
-        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -9669,6 +9693,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:A70"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
@@ -9681,18 +9717,6 @@
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
# adding scores for 17th may
</commit_message>
<xml_diff>
--- a/02062025-delhi-aiims-bsc-nursing-prepatory-data-set.xlsx
+++ b/02062025-delhi-aiims-bsc-nursing-prepatory-data-set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Github\student_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40D670F-0A20-49AC-83E4-FD3A96F93C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C33E736-9579-488B-80F5-D64AC82EC923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A5A00A1E-0852-4B43-B760-DC16954E0468}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
   <si>
     <t>date</t>
   </si>
@@ -6478,7 +6478,7 @@
   <dimension ref="A1:Q73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7913,38 +7913,48 @@
       <c r="B29" s="4">
         <v>45794</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="7" t="str">
+      <c r="C29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="5">
+        <v>48</v>
+      </c>
+      <c r="E29" s="5">
+        <v>43</v>
+      </c>
+      <c r="F29" s="5">
+        <v>2</v>
+      </c>
+      <c r="G29" s="5">
+        <v>3</v>
+      </c>
+      <c r="H29" s="7">
         <f t="shared" si="9"/>
-        <v/>
+        <v>42.333333333333336</v>
       </c>
       <c r="I29" s="5">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="J29" s="7" t="e">
+        <v>48</v>
+      </c>
+      <c r="J29" s="7">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K29" s="7" t="e">
+        <v>88.194444444444457</v>
+      </c>
+      <c r="K29" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L29" s="6" t="e">
+        <v>26.458333333333336</v>
+      </c>
+      <c r="L29" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M29" s="6" t="e">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="M29" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N29" s="6" t="e">
+        <v>0.9375</v>
+      </c>
+      <c r="N29" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
@@ -7952,38 +7962,48 @@
       <c r="B30" s="4">
         <v>45794</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="7" t="str">
+      <c r="C30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="5">
+        <v>25</v>
+      </c>
+      <c r="E30" s="5">
+        <v>25</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="7">
         <f t="shared" ref="H30:H31" si="11">IF(AND(ISNUMBER(E30), ISNUMBER(F30), ISNUMBER(G30)), E30 - (F30* 1/3), "")</f>
-        <v/>
+        <v>25</v>
       </c>
       <c r="I30" s="5">
         <f t="shared" ref="I30:I31" si="12">D30*1</f>
+        <v>25</v>
+      </c>
+      <c r="J30" s="7">
+        <f t="shared" ref="J30:J31" si="13">(H30/I30)*100</f>
+        <v>100</v>
+      </c>
+      <c r="K30" s="7">
+        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
+        <v>30</v>
+      </c>
+      <c r="L30" s="6">
+        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
+        <v>1</v>
+      </c>
+      <c r="M30" s="6">
+        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
+        <v>1</v>
+      </c>
+      <c r="N30" s="6">
+        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
         <v>0</v>
-      </c>
-      <c r="J30" s="7" t="e">
-        <f t="shared" ref="J30:J31" si="13">(H30/I30)*100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K30" s="7" t="e">
-        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L30" s="6" t="e">
-        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M30" s="6" t="e">
-        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N30" s="6" t="e">
-        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
@@ -7991,38 +8011,48 @@
       <c r="B31" s="4">
         <v>45794</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="7" t="str">
+      <c r="C31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="5">
+        <v>50</v>
+      </c>
+      <c r="E31" s="5">
+        <v>48</v>
+      </c>
+      <c r="F31" s="5">
+        <v>1</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
+      <c r="H31" s="7">
         <f t="shared" si="11"/>
-        <v/>
+        <v>47.666666666666664</v>
       </c>
       <c r="I31" s="5">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J31" s="7" t="e">
+        <v>50</v>
+      </c>
+      <c r="J31" s="7">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K31" s="7" t="e">
+        <v>95.333333333333329</v>
+      </c>
+      <c r="K31" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L31" s="6" t="e">
+        <v>28.599999999999998</v>
+      </c>
+      <c r="L31" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M31" s="6" t="e">
+        <v>0.96</v>
+      </c>
+      <c r="M31" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N31" s="6" t="e">
+        <v>0.98</v>
+      </c>
+      <c r="N31" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
@@ -9693,6 +9723,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A34"/>
     <mergeCell ref="A71:A73"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A41:A43"/>
@@ -9705,18 +9747,6 @@
     <mergeCell ref="A62:A64"/>
     <mergeCell ref="A65:A67"/>
     <mergeCell ref="A68:A70"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
updates marks for 17th, 18th and 19th (only bio)
</commit_message>
<xml_diff>
--- a/02062025-delhi-aiims-bsc-nursing-prepatory-data-set.xlsx
+++ b/02062025-delhi-aiims-bsc-nursing-prepatory-data-set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Github\student_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C33E736-9579-488B-80F5-D64AC82EC923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEAD891-0C60-427A-83E7-A0B1578B2D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A5A00A1E-0852-4B43-B760-DC16954E0468}"/>
+    <workbookView xWindow="8472" yWindow="0" windowWidth="14568" windowHeight="12240" xr2:uid="{A5A00A1E-0852-4B43-B760-DC16954E0468}"/>
   </bookViews>
   <sheets>
     <sheet name="Marksheet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
   <si>
     <t>date</t>
   </si>
@@ -6477,8 +6477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345E9B88-8FA7-480F-BC36-23D2BE33213E}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8062,38 +8062,48 @@
       <c r="B32" s="4">
         <v>45795</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="7" t="str">
+      <c r="C32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="5">
+        <v>30</v>
+      </c>
+      <c r="E32" s="5">
+        <v>28</v>
+      </c>
+      <c r="F32" s="5">
+        <v>2</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0</v>
+      </c>
+      <c r="H32" s="7">
         <f>IF(AND(ISNUMBER(E32), ISNUMBER(F32), ISNUMBER(G32)), E32 - (F32* 1/3), "")</f>
-        <v/>
+        <v>27.333333333333332</v>
       </c>
       <c r="I32" s="5">
         <f>D32*1</f>
-        <v>0</v>
-      </c>
-      <c r="J32" s="7" t="e">
+        <v>30</v>
+      </c>
+      <c r="J32" s="7">
         <f>(H32/I32)*100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K32" s="7" t="e">
+        <v>91.111111111111114</v>
+      </c>
+      <c r="K32" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L32" s="6" t="e">
+        <v>27.333333333333332</v>
+      </c>
+      <c r="L32" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M32" s="6" t="e">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="M32" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N32" s="6" t="e">
+        <v>1</v>
+      </c>
+      <c r="N32" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
@@ -8101,38 +8111,48 @@
       <c r="B33" s="4">
         <v>45795</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="7" t="str">
+      <c r="C33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="5">
+        <v>35</v>
+      </c>
+      <c r="E33" s="5">
+        <v>29</v>
+      </c>
+      <c r="F33" s="5">
+        <v>3</v>
+      </c>
+      <c r="G33" s="5">
+        <v>3</v>
+      </c>
+      <c r="H33" s="7">
         <f t="shared" ref="H33:H34" si="14">IF(AND(ISNUMBER(E33), ISNUMBER(F33), ISNUMBER(G33)), E33 - (F33* 1/3), "")</f>
-        <v/>
+        <v>28</v>
       </c>
       <c r="I33" s="5">
         <f t="shared" ref="I33:I34" si="15">D33*1</f>
-        <v>0</v>
-      </c>
-      <c r="J33" s="7" t="e">
+        <v>35</v>
+      </c>
+      <c r="J33" s="7">
         <f t="shared" ref="J33:J34" si="16">(H33/I33)*100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K33" s="7" t="e">
+        <v>80</v>
+      </c>
+      <c r="K33" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L33" s="6" t="e">
+        <v>24</v>
+      </c>
+      <c r="L33" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M33" s="6" t="e">
+        <v>0.82857142857142863</v>
+      </c>
+      <c r="M33" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N33" s="6" t="e">
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="N33" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
+        <v>8.5714285714285715E-2</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
@@ -8140,38 +8160,48 @@
       <c r="B34" s="4">
         <v>45795</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="7" t="str">
+      <c r="C34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="5">
+        <v>50</v>
+      </c>
+      <c r="E34" s="5">
+        <v>49</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0</v>
+      </c>
+      <c r="H34" s="7">
         <f t="shared" si="14"/>
-        <v/>
+        <v>48.666666666666664</v>
       </c>
       <c r="I34" s="5">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="7" t="e">
+        <v>50</v>
+      </c>
+      <c r="J34" s="7">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K34" s="7" t="e">
+        <v>97.333333333333329</v>
+      </c>
+      <c r="K34" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L34" s="6" t="e">
+        <v>29.2</v>
+      </c>
+      <c r="L34" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M34" s="6" t="e">
+        <v>0.98</v>
+      </c>
+      <c r="M34" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N34" s="6" t="e">
+        <v>1</v>
+      </c>
+      <c r="N34" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
@@ -8181,38 +8211,48 @@
       <c r="B35" s="4">
         <v>45796</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="7" t="str">
+      <c r="C35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="5">
+        <v>25</v>
+      </c>
+      <c r="E35" s="5">
+        <v>22</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0</v>
+      </c>
+      <c r="G35" s="5">
+        <v>3</v>
+      </c>
+      <c r="H35" s="7">
         <f>IF(AND(ISNUMBER(E35), ISNUMBER(F35), ISNUMBER(G35)), E35 - (F35* 1/3), "")</f>
-        <v/>
+        <v>22</v>
       </c>
       <c r="I35" s="5">
         <f>D35*1</f>
+        <v>25</v>
+      </c>
+      <c r="J35" s="7">
+        <f>(H35/I35)*100</f>
+        <v>88</v>
+      </c>
+      <c r="K35" s="7">
+        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
+        <v>26.4</v>
+      </c>
+      <c r="L35" s="6">
+        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
+        <v>0.88</v>
+      </c>
+      <c r="M35" s="6">
+        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
+        <v>0.88</v>
+      </c>
+      <c r="N35" s="6">
+        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
         <v>0</v>
-      </c>
-      <c r="J35" s="7" t="e">
-        <f>(H35/I35)*100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K35" s="7" t="e">
-        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L35" s="6" t="e">
-        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M35" s="6" t="e">
-        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N35" s="6" t="e">
-        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
@@ -8220,38 +8260,48 @@
       <c r="B36" s="4">
         <v>45796</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="7" t="str">
+      <c r="C36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="5">
+        <v>25</v>
+      </c>
+      <c r="E36" s="5">
+        <v>25</v>
+      </c>
+      <c r="F36" s="5">
+        <v>0</v>
+      </c>
+      <c r="G36" s="5">
+        <v>0</v>
+      </c>
+      <c r="H36" s="7">
         <f t="shared" ref="H36:H37" si="17">IF(AND(ISNUMBER(E36), ISNUMBER(F36), ISNUMBER(G36)), E36 - (F36* 1/3), "")</f>
-        <v/>
+        <v>25</v>
       </c>
       <c r="I36" s="5">
         <f t="shared" ref="I36:I37" si="18">D36*1</f>
+        <v>25</v>
+      </c>
+      <c r="J36" s="7">
+        <f t="shared" ref="J36:J37" si="19">(H36/I36)*100</f>
+        <v>100</v>
+      </c>
+      <c r="K36" s="7">
+        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
+        <v>30</v>
+      </c>
+      <c r="L36" s="6">
+        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
+        <v>1</v>
+      </c>
+      <c r="M36" s="6">
+        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
+        <v>1</v>
+      </c>
+      <c r="N36" s="6">
+        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
         <v>0</v>
-      </c>
-      <c r="J36" s="7" t="e">
-        <f t="shared" ref="J36:J37" si="19">(H36/I36)*100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K36" s="7" t="e">
-        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L36" s="6" t="e">
-        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M36" s="6" t="e">
-        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N36" s="6" t="e">
-        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
@@ -8259,38 +8309,48 @@
       <c r="B37" s="4">
         <v>45796</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="7" t="str">
+      <c r="C37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="5">
+        <v>50</v>
+      </c>
+      <c r="E37" s="5">
+        <v>46</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1</v>
+      </c>
+      <c r="G37" s="5">
+        <v>3</v>
+      </c>
+      <c r="H37" s="7">
         <f t="shared" si="17"/>
-        <v/>
+        <v>45.666666666666664</v>
       </c>
       <c r="I37" s="5">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="7" t="e">
+        <v>50</v>
+      </c>
+      <c r="J37" s="7">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K37" s="7" t="e">
+        <v>91.333333333333329</v>
+      </c>
+      <c r="K37" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L37" s="6" t="e">
+        <v>27.4</v>
+      </c>
+      <c r="L37" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M37" s="6" t="e">
+        <v>0.92</v>
+      </c>
+      <c r="M37" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N37" s="6" t="e">
+        <v>0.94</v>
+      </c>
+      <c r="N37" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
@@ -8300,7 +8360,9 @@
       <c r="B38" s="4">
         <v>45797</v>
       </c>
-      <c r="C38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -8339,7 +8401,9 @@
       <c r="B39" s="4">
         <v>45797</v>
       </c>
-      <c r="C39" s="5"/>
+      <c r="C39" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -8378,38 +8442,48 @@
       <c r="B40" s="4">
         <v>45797</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="7" t="str">
+      <c r="C40" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="5">
+        <v>50</v>
+      </c>
+      <c r="E40" s="5">
+        <v>44</v>
+      </c>
+      <c r="F40" s="5">
+        <v>3</v>
+      </c>
+      <c r="G40" s="5">
+        <v>3</v>
+      </c>
+      <c r="H40" s="7">
         <f>IF(AND(ISNUMBER(E40), ISNUMBER(F40), ISNUMBER(G40)), E40 - (F40* 1/3), "")</f>
-        <v/>
+        <v>43</v>
       </c>
       <c r="I40" s="5">
         <f>D40*1</f>
-        <v>0</v>
-      </c>
-      <c r="J40" s="7" t="e">
+        <v>50</v>
+      </c>
+      <c r="J40" s="7">
         <f>(H40/I40)*100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K40" s="7" t="e">
+        <v>86</v>
+      </c>
+      <c r="K40" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L40" s="6" t="e">
+        <v>25.8</v>
+      </c>
+      <c r="L40" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M40" s="6" t="e">
+        <v>0.88</v>
+      </c>
+      <c r="M40" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N40" s="6" t="e">
+        <v>0.94</v>
+      </c>
+      <c r="N40" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
@@ -9723,6 +9797,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:A70"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
@@ -9735,18 +9821,6 @@
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
updated the incorrect scores and added the complete 22nd may marks
</commit_message>
<xml_diff>
--- a/02062025-delhi-aiims-bsc-nursing-prepatory-data-set.xlsx
+++ b/02062025-delhi-aiims-bsc-nursing-prepatory-data-set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Github\student_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B9FEA5-A719-4EAD-9D86-1447B47C75DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF805CC-DEEA-4418-AE69-1A18FBA291FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A5A00A1E-0852-4B43-B760-DC16954E0468}"/>
   </bookViews>
@@ -6477,8 +6477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345E9B88-8FA7-480F-BC36-23D2BE33213E}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8711,44 +8711,44 @@
         <v>9</v>
       </c>
       <c r="D45" s="5">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E45" s="5">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F45" s="5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G45" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H45" s="7">
-        <f t="shared" ref="H45:H46" si="23">IF(AND(ISNUMBER(E45), ISNUMBER(F45), ISNUMBER(G45)), E45 - (F45* 1/3), "")</f>
-        <v>47</v>
+        <f>IF(AND(ISNUMBER(E45), ISNUMBER(F45), ISNUMBER(G45)), E45 - (F45* 1/3), "")</f>
+        <v>49</v>
       </c>
       <c r="I45" s="5">
-        <f t="shared" ref="I45:I46" si="24">D45*1</f>
-        <v>50</v>
+        <f>D45*1</f>
+        <v>61</v>
       </c>
       <c r="J45" s="7">
-        <f t="shared" ref="J45:J46" si="25">(H45/I45)*100</f>
-        <v>94</v>
+        <f t="shared" ref="J45:J46" si="23">(H45/I45)*100</f>
+        <v>80.327868852459019</v>
       </c>
       <c r="K45" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>28.2</v>
+        <v>24.098360655737704</v>
       </c>
       <c r="L45" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>0.94</v>
+        <v>0.83606557377049184</v>
       </c>
       <c r="M45" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>0.94</v>
+        <v>0.93442622950819676</v>
       </c>
       <c r="N45" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>0</v>
+        <v>9.8360655737704916E-2</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
@@ -8759,37 +8759,45 @@
       <c r="C46" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="7" t="str">
+      <c r="D46" s="5">
+        <v>50</v>
+      </c>
+      <c r="E46" s="5">
+        <v>47</v>
+      </c>
+      <c r="F46" s="5">
+        <v>0</v>
+      </c>
+      <c r="G46" s="5">
+        <v>3</v>
+      </c>
+      <c r="H46" s="7">
+        <f>IF(AND(ISNUMBER(E46), ISNUMBER(F46), ISNUMBER(G46)), E46 - (F46* 1/3), "")</f>
+        <v>47</v>
+      </c>
+      <c r="I46" s="5">
+        <f>D46*1</f>
+        <v>50</v>
+      </c>
+      <c r="J46" s="7">
         <f t="shared" si="23"/>
-        <v/>
-      </c>
-      <c r="I46" s="5">
-        <f t="shared" si="24"/>
+        <v>94</v>
+      </c>
+      <c r="K46" s="7">
+        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
+        <v>28.2</v>
+      </c>
+      <c r="L46" s="6">
+        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
+        <v>0.94</v>
+      </c>
+      <c r="M46" s="6">
+        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
+        <v>0.94</v>
+      </c>
+      <c r="N46" s="6">
+        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
         <v>0</v>
-      </c>
-      <c r="J46" s="7" t="e">
-        <f t="shared" si="25"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K46" s="7" t="e">
-        <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L46" s="6" t="e">
-        <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M46" s="6" t="e">
-        <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N46" s="6" t="e">
-        <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
@@ -8843,45 +8851,37 @@
       <c r="C48" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="5">
-        <v>61</v>
-      </c>
-      <c r="E48" s="5">
-        <v>51</v>
-      </c>
-      <c r="F48" s="5">
-        <v>6</v>
-      </c>
-      <c r="G48" s="5">
-        <v>4</v>
-      </c>
-      <c r="H48" s="7">
-        <f t="shared" ref="H48:H49" si="26">IF(AND(ISNUMBER(E48), ISNUMBER(F48), ISNUMBER(G48)), E48 - (F48* 1/3), "")</f>
-        <v>49</v>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="7" t="str">
+        <f>IF(AND(ISNUMBER(E48), ISNUMBER(F48), ISNUMBER(G48)), E48 - (F48* 1/3), "")</f>
+        <v/>
       </c>
       <c r="I48" s="5">
-        <f t="shared" ref="I48:I49" si="27">D48*1</f>
-        <v>61</v>
-      </c>
-      <c r="J48" s="7">
-        <f t="shared" ref="J48:J49" si="28">(H48/I48)*100</f>
-        <v>80.327868852459019</v>
-      </c>
-      <c r="K48" s="7">
+        <f>D48*1</f>
+        <v>0</v>
+      </c>
+      <c r="J48" s="7" t="e">
+        <f t="shared" ref="J48:J49" si="24">(H48/I48)*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K48" s="7" t="e">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>24.098360655737704</v>
-      </c>
-      <c r="L48" s="6">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L48" s="6" t="e">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>0.83606557377049184</v>
-      </c>
-      <c r="M48" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M48" s="6" t="e">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>0.93442622950819676</v>
-      </c>
-      <c r="N48" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N48" s="6" t="e">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>9.8360655737704916E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
@@ -8897,15 +8897,15 @@
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="7" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="H48:H49" si="25">IF(AND(ISNUMBER(E49), ISNUMBER(F49), ISNUMBER(G49)), E49 - (F49* 1/3), "")</f>
         <v/>
       </c>
       <c r="I49" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="I48:I49" si="26">D49*1</f>
         <v>0</v>
       </c>
       <c r="J49" s="7" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="K49" s="7" t="e">
@@ -8981,15 +8981,15 @@
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="7" t="str">
-        <f t="shared" ref="H51:H52" si="29">IF(AND(ISNUMBER(E51), ISNUMBER(F51), ISNUMBER(G51)), E51 - (F51* 1/3), "")</f>
+        <f t="shared" ref="H51:H52" si="27">IF(AND(ISNUMBER(E51), ISNUMBER(F51), ISNUMBER(G51)), E51 - (F51* 1/3), "")</f>
         <v/>
       </c>
       <c r="I51" s="5">
-        <f t="shared" ref="I51:I52" si="30">D51*1</f>
+        <f t="shared" ref="I51:I52" si="28">D51*1</f>
         <v>0</v>
       </c>
       <c r="J51" s="7" t="e">
-        <f t="shared" ref="J51:J52" si="31">(H51/I51)*100</f>
+        <f t="shared" ref="J51:J52" si="29">(H51/I51)*100</f>
         <v>#VALUE!</v>
       </c>
       <c r="K51" s="7" t="e">
@@ -9022,15 +9022,15 @@
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="7" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="I52" s="5">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="J52" s="7" t="e">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="I52" s="5">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="J52" s="7" t="e">
-        <f t="shared" si="31"/>
         <v>#VALUE!</v>
       </c>
       <c r="K52" s="7" t="e">
@@ -9106,15 +9106,15 @@
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="7" t="str">
-        <f t="shared" ref="H54:H55" si="32">IF(AND(ISNUMBER(E54), ISNUMBER(F54), ISNUMBER(G54)), E54 - (F54* 1/3), "")</f>
+        <f t="shared" ref="H54:H55" si="30">IF(AND(ISNUMBER(E54), ISNUMBER(F54), ISNUMBER(G54)), E54 - (F54* 1/3), "")</f>
         <v/>
       </c>
       <c r="I54" s="5">
-        <f t="shared" ref="I54:I55" si="33">D54*1</f>
+        <f t="shared" ref="I54:I55" si="31">D54*1</f>
         <v>0</v>
       </c>
       <c r="J54" s="7" t="e">
-        <f t="shared" ref="J54:J55" si="34">(H54/I54)*100</f>
+        <f t="shared" ref="J54:J55" si="32">(H54/I54)*100</f>
         <v>#VALUE!</v>
       </c>
       <c r="K54" s="7" t="e">
@@ -9147,15 +9147,15 @@
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="7" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+      <c r="I55" s="5">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="J55" s="7" t="e">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="I55" s="5">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="J55" s="7" t="e">
-        <f t="shared" si="34"/>
         <v>#VALUE!</v>
       </c>
       <c r="K55" s="7" t="e">
@@ -9231,15 +9231,15 @@
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="7" t="str">
-        <f t="shared" ref="H57:H58" si="35">IF(AND(ISNUMBER(E57), ISNUMBER(F57), ISNUMBER(G57)), E57 - (F57* 1/3), "")</f>
+        <f t="shared" ref="H57:H58" si="33">IF(AND(ISNUMBER(E57), ISNUMBER(F57), ISNUMBER(G57)), E57 - (F57* 1/3), "")</f>
         <v/>
       </c>
       <c r="I57" s="5">
-        <f t="shared" ref="I57:I58" si="36">D57*1</f>
+        <f t="shared" ref="I57:I58" si="34">D57*1</f>
         <v>0</v>
       </c>
       <c r="J57" s="7" t="e">
-        <f t="shared" ref="J57:J58" si="37">(H57/I57)*100</f>
+        <f t="shared" ref="J57:J58" si="35">(H57/I57)*100</f>
         <v>#VALUE!</v>
       </c>
       <c r="K57" s="7" t="e">
@@ -9272,15 +9272,15 @@
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="7" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="I58" s="5">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="J58" s="7" t="e">
         <f t="shared" si="35"/>
-        <v/>
-      </c>
-      <c r="I58" s="5">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="J58" s="7" t="e">
-        <f t="shared" si="37"/>
         <v>#VALUE!</v>
       </c>
       <c r="K58" s="7" t="e">
@@ -9356,15 +9356,15 @@
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="7" t="str">
-        <f t="shared" ref="H60:H61" si="38">IF(AND(ISNUMBER(E60), ISNUMBER(F60), ISNUMBER(G60)), E60 - (F60* 1/3), "")</f>
+        <f t="shared" ref="H60:H61" si="36">IF(AND(ISNUMBER(E60), ISNUMBER(F60), ISNUMBER(G60)), E60 - (F60* 1/3), "")</f>
         <v/>
       </c>
       <c r="I60" s="5">
-        <f t="shared" ref="I60:I61" si="39">D60*1</f>
+        <f t="shared" ref="I60:I61" si="37">D60*1</f>
         <v>0</v>
       </c>
       <c r="J60" s="7" t="e">
-        <f t="shared" ref="J60:J61" si="40">(H60/I60)*100</f>
+        <f t="shared" ref="J60:J61" si="38">(H60/I60)*100</f>
         <v>#VALUE!</v>
       </c>
       <c r="K60" s="7" t="e">
@@ -9397,15 +9397,15 @@
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="7" t="str">
+        <f t="shared" si="36"/>
+        <v/>
+      </c>
+      <c r="I61" s="5">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="J61" s="7" t="e">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="I61" s="5">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="J61" s="7" t="e">
-        <f t="shared" si="40"/>
         <v>#VALUE!</v>
       </c>
       <c r="K61" s="7" t="e">
@@ -9481,15 +9481,15 @@
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="7" t="str">
-        <f t="shared" ref="H63:H64" si="41">IF(AND(ISNUMBER(E63), ISNUMBER(F63), ISNUMBER(G63)), E63 - (F63* 1/3), "")</f>
+        <f t="shared" ref="H63:H64" si="39">IF(AND(ISNUMBER(E63), ISNUMBER(F63), ISNUMBER(G63)), E63 - (F63* 1/3), "")</f>
         <v/>
       </c>
       <c r="I63" s="5">
-        <f t="shared" ref="I63:I64" si="42">D63*1</f>
+        <f t="shared" ref="I63:I64" si="40">D63*1</f>
         <v>0</v>
       </c>
       <c r="J63" s="7" t="e">
-        <f t="shared" ref="J63:J64" si="43">(H63/I63)*100</f>
+        <f t="shared" ref="J63:J64" si="41">(H63/I63)*100</f>
         <v>#VALUE!</v>
       </c>
       <c r="K63" s="7" t="e">
@@ -9522,15 +9522,15 @@
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="7" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="I64" s="5">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J64" s="7" t="e">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="I64" s="5">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="J64" s="7" t="e">
-        <f t="shared" si="43"/>
         <v>#VALUE!</v>
       </c>
       <c r="K64" s="7" t="e">
@@ -9606,15 +9606,15 @@
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
       <c r="H66" s="7" t="str">
-        <f t="shared" ref="H66:H67" si="44">IF(AND(ISNUMBER(E66), ISNUMBER(F66), ISNUMBER(G66)), E66 - (F66* 1/3), "")</f>
+        <f t="shared" ref="H66:H67" si="42">IF(AND(ISNUMBER(E66), ISNUMBER(F66), ISNUMBER(G66)), E66 - (F66* 1/3), "")</f>
         <v/>
       </c>
       <c r="I66" s="5">
-        <f t="shared" ref="I66:I67" si="45">D66*1</f>
+        <f t="shared" ref="I66:I67" si="43">D66*1</f>
         <v>0</v>
       </c>
       <c r="J66" s="7" t="e">
-        <f t="shared" ref="J66:J67" si="46">(H66/I66)*100</f>
+        <f t="shared" ref="J66:J67" si="44">(H66/I66)*100</f>
         <v>#VALUE!</v>
       </c>
       <c r="K66" s="7" t="e">
@@ -9647,15 +9647,15 @@
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="7" t="str">
+        <f t="shared" si="42"/>
+        <v/>
+      </c>
+      <c r="I67" s="5">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="J67" s="7" t="e">
         <f t="shared" si="44"/>
-        <v/>
-      </c>
-      <c r="I67" s="5">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="J67" s="7" t="e">
-        <f t="shared" si="46"/>
         <v>#VALUE!</v>
       </c>
       <c r="K67" s="7" t="e">
@@ -9690,15 +9690,15 @@
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="H68" s="7" t="str">
-        <f t="shared" ref="H68:H73" si="47">IF(AND(ISNUMBER(E68), ISNUMBER(F68), ISNUMBER(G68)), E68 - (F68* 1/3), "")</f>
+        <f t="shared" ref="H68:H73" si="45">IF(AND(ISNUMBER(E68), ISNUMBER(F68), ISNUMBER(G68)), E68 - (F68* 1/3), "")</f>
         <v/>
       </c>
       <c r="I68" s="5">
-        <f t="shared" ref="I68:I73" si="48">D68*1</f>
+        <f t="shared" ref="I68:I73" si="46">D68*1</f>
         <v>0</v>
       </c>
       <c r="J68" s="7" t="e">
-        <f t="shared" ref="J68:J73" si="49">(H68/I68)*100</f>
+        <f t="shared" ref="J68:J73" si="47">(H68/I68)*100</f>
         <v>#VALUE!</v>
       </c>
       <c r="K68" s="7" t="e">
@@ -9731,15 +9731,15 @@
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="H69" s="7" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="I69" s="5">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="J69" s="7" t="e">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="I69" s="5">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="J69" s="7" t="e">
-        <f t="shared" si="49"/>
         <v>#VALUE!</v>
       </c>
       <c r="K69" s="7" t="e">
@@ -9772,15 +9772,15 @@
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="7" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="I70" s="5">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="J70" s="7" t="e">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="I70" s="5">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="J70" s="7" t="e">
-        <f t="shared" si="49"/>
         <v>#VALUE!</v>
       </c>
       <c r="K70" s="7" t="e">
@@ -9815,15 +9815,15 @@
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
       <c r="H71" s="7" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="I71" s="5">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="J71" s="7" t="e">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="I71" s="5">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="J71" s="7" t="e">
-        <f t="shared" si="49"/>
         <v>#VALUE!</v>
       </c>
       <c r="K71" s="7" t="e">
@@ -9856,15 +9856,15 @@
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
       <c r="H72" s="7" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="I72" s="5">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="J72" s="7" t="e">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="I72" s="5">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="J72" s="7" t="e">
-        <f t="shared" si="49"/>
         <v>#VALUE!</v>
       </c>
       <c r="K72" s="7" t="e">
@@ -9897,15 +9897,15 @@
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="7" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="I73" s="5">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="J73" s="7" t="e">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="I73" s="5">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="J73" s="7" t="e">
-        <f t="shared" si="49"/>
         <v>#VALUE!</v>
       </c>
       <c r="K73" s="7" t="e">
@@ -9927,6 +9927,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A34"/>
     <mergeCell ref="A71:A73"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A41:A43"/>
@@ -9939,18 +9951,6 @@
     <mergeCell ref="A62:A64"/>
     <mergeCell ref="A65:A67"/>
     <mergeCell ref="A68:A70"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added marks for 26-05-2025
</commit_message>
<xml_diff>
--- a/02062025-delhi-aiims-bsc-nursing-prepatory-data-set.xlsx
+++ b/02062025-delhi-aiims-bsc-nursing-prepatory-data-set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Github\student_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40D1423-A129-4090-9FB5-174E92414CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC6C330-4464-471F-8E89-0761C49C8E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A5A00A1E-0852-4B43-B760-DC16954E0468}"/>
   </bookViews>
@@ -6477,8 +6477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345E9B88-8FA7-480F-BC36-23D2BE33213E}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="113" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6555,20 +6555,21 @@
         <v>7</v>
       </c>
       <c r="D2" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>100</v>
       </c>
       <c r="E2" s="5">
         <v>68</v>
       </c>
       <c r="F2" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="5">
         <v>17</v>
       </c>
       <c r="H2" s="7">
         <f>IF(AND(ISNUMBER(E2), ISNUMBER(F2), ISNUMBER(G2)), E2 - (F2* 1/3), "")</f>
-        <v>63.333333333333336</v>
+        <v>63</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2:I20" si="0">D2*1</f>
@@ -6576,11 +6577,11 @@
       </c>
       <c r="J2" s="7">
         <f>(H2/I2)*100</f>
-        <v>63.333333333333329</v>
+        <v>63</v>
       </c>
       <c r="K2" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>19</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="L2" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
@@ -6588,11 +6589,11 @@
       </c>
       <c r="M2" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>0.82</v>
+        <v>0.83</v>
       </c>
       <c r="N2" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -6604,6 +6605,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>37</v>
       </c>
       <c r="E3" s="5">
@@ -6660,6 +6662,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>30</v>
       </c>
       <c r="E4" s="5">
@@ -6704,7 +6707,7 @@
       </c>
       <c r="Q4" s="10">
         <f>AVERAGE(M2:M16)</f>
-        <v>0.91119676269676286</v>
+        <v>0.91186342936342935</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -6717,7 +6720,8 @@
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>32</v>
       </c>
       <c r="E5" s="5">
@@ -6762,7 +6766,7 @@
       </c>
       <c r="Q5" s="10">
         <f>AVERAGE(N2:N16)</f>
-        <v>7.0107005357005356E-2</v>
+        <v>7.0773672023672018E-2</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -6774,6 +6778,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>26</v>
       </c>
       <c r="E6" s="5">
@@ -6823,6 +6828,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>30</v>
       </c>
       <c r="E7" s="5">
@@ -6874,6 +6880,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>36</v>
       </c>
       <c r="E8" s="5">
@@ -6923,6 +6930,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>42</v>
       </c>
       <c r="E9" s="5">
@@ -6972,6 +6980,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E10" s="5">
@@ -7023,6 +7032,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>26</v>
       </c>
       <c r="E11" s="5">
@@ -7072,6 +7082,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>42</v>
       </c>
       <c r="E12" s="5">
@@ -7121,6 +7132,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E13" s="5">
@@ -7172,6 +7184,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>30</v>
       </c>
       <c r="E14" s="5">
@@ -7221,6 +7234,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>42</v>
       </c>
       <c r="E15" s="5">
@@ -7270,6 +7284,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E16" s="5">
@@ -7321,6 +7336,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>54</v>
       </c>
       <c r="E17" s="5">
@@ -7370,7 +7386,8 @@
         <v>9</v>
       </c>
       <c r="D18" s="5">
-        <v>62</v>
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
+        <v>61</v>
       </c>
       <c r="E18" s="5">
         <v>50</v>
@@ -7387,27 +7404,27 @@
       </c>
       <c r="I18" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" si="4"/>
-        <v>76.881720430107521</v>
+        <v>78.142076502732237</v>
       </c>
       <c r="K18" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>23.064516129032256</v>
+        <v>23.442622950819672</v>
       </c>
       <c r="L18" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>0.80645161290322576</v>
+        <v>0.81967213114754101</v>
       </c>
       <c r="M18" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>0.91935483870967738</v>
+        <v>0.93442622950819676</v>
       </c>
       <c r="N18" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>0.11290322580645161</v>
+        <v>0.11475409836065574</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -7419,6 +7436,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E19" s="5">
@@ -7470,6 +7488,7 @@
         <v>7</v>
       </c>
       <c r="D20" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>27</v>
       </c>
       <c r="E20" s="5">
@@ -7519,6 +7538,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>55</v>
       </c>
       <c r="E21" s="5">
@@ -7568,6 +7588,7 @@
         <v>8</v>
       </c>
       <c r="D22" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E22" s="5">
@@ -7619,6 +7640,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>24</v>
       </c>
       <c r="E23" s="5">
@@ -7668,6 +7690,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>18</v>
       </c>
       <c r="E24" s="5">
@@ -7717,6 +7740,7 @@
         <v>8</v>
       </c>
       <c r="D25" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E25" s="5">
@@ -7768,6 +7792,7 @@
         <v>7</v>
       </c>
       <c r="D26" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>45</v>
       </c>
       <c r="E26" s="5">
@@ -7817,6 +7842,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>25</v>
       </c>
       <c r="E27" s="5">
@@ -7866,6 +7892,7 @@
         <v>8</v>
       </c>
       <c r="D28" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E28" s="5">
@@ -7917,6 +7944,7 @@
         <v>7</v>
       </c>
       <c r="D29" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>48</v>
       </c>
       <c r="E29" s="5">
@@ -7966,6 +7994,7 @@
         <v>9</v>
       </c>
       <c r="D30" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>25</v>
       </c>
       <c r="E30" s="5">
@@ -8015,6 +8044,7 @@
         <v>8</v>
       </c>
       <c r="D31" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E31" s="5">
@@ -8066,6 +8096,7 @@
         <v>7</v>
       </c>
       <c r="D32" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>30</v>
       </c>
       <c r="E32" s="5">
@@ -8115,6 +8146,7 @@
         <v>9</v>
       </c>
       <c r="D33" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>35</v>
       </c>
       <c r="E33" s="5">
@@ -8164,6 +8196,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E34" s="5">
@@ -8215,6 +8248,7 @@
         <v>7</v>
       </c>
       <c r="D35" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>25</v>
       </c>
       <c r="E35" s="5">
@@ -8264,6 +8298,7 @@
         <v>9</v>
       </c>
       <c r="D36" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>25</v>
       </c>
       <c r="E36" s="5">
@@ -8313,6 +8348,7 @@
         <v>8</v>
       </c>
       <c r="D37" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E37" s="5">
@@ -8364,6 +8400,7 @@
         <v>7</v>
       </c>
       <c r="D38" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>45</v>
       </c>
       <c r="E38" s="5">
@@ -8413,6 +8450,7 @@
         <v>9</v>
       </c>
       <c r="D39" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>65</v>
       </c>
       <c r="E39" s="5">
@@ -8462,6 +8500,7 @@
         <v>8</v>
       </c>
       <c r="D40" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E40" s="5">
@@ -8513,6 +8552,7 @@
         <v>7</v>
       </c>
       <c r="D41" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>63</v>
       </c>
       <c r="E41" s="5">
@@ -8562,6 +8602,7 @@
         <v>9</v>
       </c>
       <c r="D42" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>18</v>
       </c>
       <c r="E42" s="5">
@@ -8611,6 +8652,7 @@
         <v>8</v>
       </c>
       <c r="D43" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E43" s="5">
@@ -8662,6 +8704,7 @@
         <v>7</v>
       </c>
       <c r="D44" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>74</v>
       </c>
       <c r="E44" s="5">
@@ -8711,6 +8754,7 @@
         <v>9</v>
       </c>
       <c r="D45" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>61</v>
       </c>
       <c r="E45" s="5">
@@ -8760,6 +8804,7 @@
         <v>8</v>
       </c>
       <c r="D46" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E46" s="5">
@@ -8811,6 +8856,7 @@
         <v>7</v>
       </c>
       <c r="D47" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>19</v>
       </c>
       <c r="E47" s="5">
@@ -8860,6 +8906,7 @@
         <v>9</v>
       </c>
       <c r="D48" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>25</v>
       </c>
       <c r="E48" s="5">
@@ -8909,6 +8956,7 @@
         <v>8</v>
       </c>
       <c r="D49" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E49" s="5">
@@ -8960,6 +9008,7 @@
         <v>7</v>
       </c>
       <c r="D50" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>29</v>
       </c>
       <c r="E50" s="5">
@@ -9009,6 +9058,7 @@
         <v>9</v>
       </c>
       <c r="D51" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>72</v>
       </c>
       <c r="E51" s="5">
@@ -9058,6 +9108,7 @@
         <v>8</v>
       </c>
       <c r="D52" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E52" s="5">
@@ -9109,6 +9160,7 @@
         <v>7</v>
       </c>
       <c r="D53" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>37</v>
       </c>
       <c r="E53" s="5">
@@ -9158,6 +9210,7 @@
         <v>9</v>
       </c>
       <c r="D54" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>22</v>
       </c>
       <c r="E54" s="5">
@@ -9207,6 +9260,7 @@
         <v>8</v>
       </c>
       <c r="D55" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
         <v>50</v>
       </c>
       <c r="E55" s="5">
@@ -9257,37 +9311,46 @@
       <c r="C56" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="7" t="str">
+      <c r="D56" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
+        <v>50</v>
+      </c>
+      <c r="E56" s="5">
+        <v>47</v>
+      </c>
+      <c r="F56" s="5">
+        <v>2</v>
+      </c>
+      <c r="G56" s="5">
+        <v>1</v>
+      </c>
+      <c r="H56" s="7">
         <f>IF(AND(ISNUMBER(E56), ISNUMBER(F56), ISNUMBER(G56)), E56 - (F56* 1/3), "")</f>
-        <v/>
+        <v>46.333333333333336</v>
       </c>
       <c r="I56" s="5">
         <f>D56*1</f>
-        <v>0</v>
-      </c>
-      <c r="J56" s="7" t="e">
+        <v>50</v>
+      </c>
+      <c r="J56" s="7">
         <f>(H56/I56)*100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K56" s="7" t="e">
+        <v>92.666666666666671</v>
+      </c>
+      <c r="K56" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L56" s="6" t="e">
+        <v>27.800000000000004</v>
+      </c>
+      <c r="L56" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M56" s="6" t="e">
+        <v>0.94</v>
+      </c>
+      <c r="M56" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N56" s="6" t="e">
+        <v>0.98</v>
+      </c>
+      <c r="N56" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
@@ -9298,37 +9361,46 @@
       <c r="C57" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="7" t="str">
+      <c r="D57" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
+        <v>21</v>
+      </c>
+      <c r="E57" s="5">
+        <v>19</v>
+      </c>
+      <c r="F57" s="5">
+        <v>2</v>
+      </c>
+      <c r="G57" s="5">
+        <v>0</v>
+      </c>
+      <c r="H57" s="7">
         <f t="shared" ref="H57:H58" si="33">IF(AND(ISNUMBER(E57), ISNUMBER(F57), ISNUMBER(G57)), E57 - (F57* 1/3), "")</f>
-        <v/>
+        <v>18.333333333333332</v>
       </c>
       <c r="I57" s="5">
         <f t="shared" ref="I57:I58" si="34">D57*1</f>
-        <v>0</v>
-      </c>
-      <c r="J57" s="7" t="e">
+        <v>21</v>
+      </c>
+      <c r="J57" s="7">
         <f t="shared" ref="J57:J58" si="35">(H57/I57)*100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K57" s="7" t="e">
+        <v>87.30158730158729</v>
+      </c>
+      <c r="K57" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L57" s="6" t="e">
+        <v>26.190476190476186</v>
+      </c>
+      <c r="L57" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M57" s="6" t="e">
+        <v>0.90476190476190477</v>
+      </c>
+      <c r="M57" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N57" s="6" t="e">
+        <v>1</v>
+      </c>
+      <c r="N57" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
+        <v>9.5238095238095233E-2</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
@@ -9339,37 +9411,46 @@
       <c r="C58" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="7" t="str">
+      <c r="D58" s="5">
+        <f>SUM(Table1[[#This Row],[correct]:[unattempted]])</f>
+        <v>50</v>
+      </c>
+      <c r="E58" s="5">
+        <v>47</v>
+      </c>
+      <c r="F58" s="5">
+        <v>3</v>
+      </c>
+      <c r="G58" s="5">
+        <v>0</v>
+      </c>
+      <c r="H58" s="7">
         <f t="shared" si="33"/>
-        <v/>
+        <v>46</v>
       </c>
       <c r="I58" s="5">
         <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="J58" s="7" t="e">
+        <v>50</v>
+      </c>
+      <c r="J58" s="7">
         <f t="shared" si="35"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K58" s="7" t="e">
+        <v>92</v>
+      </c>
+      <c r="K58" s="7">
         <f>(Table1[[#This Row],[marks]]/Table1[[#This Row],[total]])*30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L58" s="6" t="e">
+        <v>27.6</v>
+      </c>
+      <c r="L58" s="6">
         <f>Table1[[#This Row],[correct]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M58" s="6" t="e">
+        <v>0.94</v>
+      </c>
+      <c r="M58" s="6">
         <f>(Table1[[#This Row],[correct]]+Table1[[#This Row],[incorrect]])/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N58" s="6" t="e">
+        <v>1</v>
+      </c>
+      <c r="N58" s="6">
         <f>Table1[[#This Row],[incorrect]]/Table1[[#This Row],[total]]</f>
-        <v>#DIV/0!</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.3">
@@ -9999,6 +10080,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="A68:A70"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
@@ -10011,18 +10104,6 @@
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>